<commit_message>
changes for round 10 mainly involving handling of team names
</commit_message>
<xml_diff>
--- a/data/inputs/adhoc_changes.xlsx
+++ b/data/inputs/adhoc_changes.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.thomas\Desktop\Michael Thomas\Moreira's Magic\mm\data\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timothy.gummer\Documents\__Personal__\mm\cloned_repos\mm\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8B9F5A-7C90-4E32-B1FE-41B6C7C30137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EE90AA-318A-4AF0-BAFF-9042F5800900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1EAA6D6E-7449-43EC-BF3B-A7990396BF95}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1EAA6D6E-7449-43EC-BF3B-A7990396BF95}"/>
   </bookViews>
   <sheets>
     <sheet name="player_id" sheetId="1" r:id="rId1"/>
     <sheet name="team_names" sheetId="3" r:id="rId2"/>
-    <sheet name="player" sheetId="2" r:id="rId3"/>
-    <sheet name="footywire" sheetId="4" r:id="rId4"/>
+    <sheet name="team_names_short" sheetId="5" r:id="rId3"/>
+    <sheet name="player" sheetId="2" r:id="rId4"/>
+    <sheet name="footywire" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="193">
   <si>
     <t>player_id</t>
   </si>
@@ -549,6 +550,75 @@
   </si>
   <si>
     <t>mm_name</t>
+  </si>
+  <si>
+    <t>Euro-Yroke</t>
+  </si>
+  <si>
+    <t>Kuwarna</t>
+  </si>
+  <si>
+    <t>Narrm</t>
+  </si>
+  <si>
+    <t>Waalitj Marawar</t>
+  </si>
+  <si>
+    <t>Walyalup</t>
+  </si>
+  <si>
+    <t>Yartapuulti</t>
+  </si>
+  <si>
+    <t>Port Adelaide</t>
+  </si>
+  <si>
+    <t>St Kilda</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>West Coast Eagles</t>
+  </si>
+  <si>
+    <t>Fremantle</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>KUW</t>
+  </si>
+  <si>
+    <t>NAR</t>
+  </si>
+  <si>
+    <t>WAA</t>
+  </si>
+  <si>
+    <t>WAL</t>
+  </si>
+  <si>
+    <t>YAR</t>
+  </si>
+  <si>
+    <t>STK</t>
+  </si>
+  <si>
+    <t>ADE</t>
+  </si>
+  <si>
+    <t>MEL</t>
+  </si>
+  <si>
+    <t>WCE</t>
+  </si>
+  <si>
+    <t>FRE</t>
+  </si>
+  <si>
+    <t>PTA</t>
   </si>
 </sst>
 </file>
@@ -906,12 +976,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="12.7109375" customWidth="1"/>
+    <col min="1" max="3" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -940,19 +1010,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFB8F58-8D80-4E97-A892-2D3E8475EBE4}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B6" sqref="B6:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -960,7 +1030,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -968,7 +1038,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -976,7 +1046,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -984,12 +1054,60 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -998,6 +1116,75 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E684ABB7-8F65-48EE-B7DF-E99BD3DAA6D1}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B4F64C-9302-4F26-8B1B-8FFEA69DC804}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -1005,15 +1192,15 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1214,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1256,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1083,7 +1270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1097,7 +1284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1111,7 +1298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1127,7 +1314,7 @@
         <v>Dodson</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1143,7 +1330,7 @@
         <v>Gerreyn</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1159,7 +1346,7 @@
         <v>Angove</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1175,7 +1362,7 @@
         <v>Smith</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1191,7 +1378,7 @@
         <v>Smillie</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1207,7 +1394,7 @@
         <v>Barrett</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1223,7 +1410,7 @@
         <v>Clarke</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1239,7 +1426,7 @@
         <v>Allan</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1255,7 +1442,7 @@
         <v>Gulbin</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1271,7 +1458,7 @@
         <v>Alger</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1287,7 +1474,7 @@
         <v>Sims</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1308,21 +1495,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4AF9C0-8E67-4C29-8B31-DC8FFDE805E2}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>169</v>
       </c>
@@ -1330,7 +1515,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>167</v>
       </c>
@@ -1338,7 +1523,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -1346,7 +1531,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1354,7 +1539,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -1362,7 +1547,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -1370,7 +1555,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -1378,7 +1563,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -1386,7 +1571,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -1394,7 +1579,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>151</v>
       </c>
@@ -1402,7 +1587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -1410,7 +1595,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -1418,7 +1603,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -1426,7 +1611,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -1434,7 +1619,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -1442,7 +1627,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -1450,7 +1635,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -1458,7 +1643,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -1466,7 +1651,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -1474,7 +1659,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -1482,7 +1667,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -1490,7 +1675,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -1498,7 +1683,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -1506,7 +1691,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -1514,7 +1699,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>122</v>
       </c>
@@ -1522,7 +1707,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -1530,7 +1715,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>118</v>
       </c>
@@ -1538,7 +1723,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>116</v>
       </c>
@@ -1546,7 +1731,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -1554,7 +1739,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -1562,7 +1747,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -1570,7 +1755,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -1578,7 +1763,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -1586,7 +1771,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -1594,7 +1779,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -1602,7 +1787,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -1610,7 +1795,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -1618,7 +1803,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -1626,7 +1811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -1634,7 +1819,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>92</v>
       </c>
@@ -1642,7 +1827,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -1650,7 +1835,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -1658,7 +1843,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1666,7 +1851,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1674,7 +1859,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -1682,7 +1867,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -1690,7 +1875,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -1698,7 +1883,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -1706,7 +1891,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -1714,7 +1899,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -1722,7 +1907,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -1730,7 +1915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>68</v>
       </c>

</xml_diff>